<commit_message>
&& - № 79032024 от 05.06.25 https://meshok.net/ - № 79031149 от 05.06.25 https://meshok.net/ - № 79031139 от 05.06.25 https://meshok.net/ - №19387 от 16.06.2025 https://2eurostore.ru/ - №18764 от 02.06.2025 https://2eurostore.ru/ - №18682 от 01.06.2025 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/Canada/#Canada#Commemorative#[2003-present]#circulation_quality.xlsx
+++ b/Collections/Canada/#Canada#Commemorative#[2003-present]#circulation_quality.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\Canada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351DB487-39BD-4C27-B874-07C854D971FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38A065F-3966-42DC-9CCB-959E3E21390F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3195,7 +3195,7 @@
       <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D45" sqref="A44:D45"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4812,7 +4812,7 @@
       <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38:D38"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5039,7 +5039,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
@@ -6035,7 +6035,7 @@
       <formula>NOT(ISERROR(SEARCH(("*-"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9 I5 I11 I13 I15 I17 I19 I21 I23">
+  <conditionalFormatting sqref="I5 I9 I11 I13 I15 I17 I19 I21 I23">
     <cfRule type="colorScale" priority="200">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -6072,7 +6072,7 @@
       <formula>NOT(ISERROR(SEARCH(("*-"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9 H5 H11 H13 H15 H17 H19 H21 H23">
+  <conditionalFormatting sqref="H5 H9 H11 H13 H15 H17 H19 H21 H23">
     <cfRule type="colorScale" priority="192">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -6104,7 +6104,7 @@
       <formula>NOT(ISERROR(SEARCH(("*-"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8 I6 I10 I12 I14 I20">
+  <conditionalFormatting sqref="I6 I8 I10 I12 I14 I20">
     <cfRule type="colorScale" priority="187">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -6141,7 +6141,7 @@
       <formula>NOT(ISERROR(SEARCH(("*-"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8 H6 H10 H12 H14 H20">
+  <conditionalFormatting sqref="H6 H8 H10 H12 H14 H20">
     <cfRule type="colorScale" priority="181">
       <colorScale>
         <cfvo type="formula" val="0"/>

</xml_diff>